<commit_message>
fix a bug of fitting
</commit_message>
<xml_diff>
--- a/logs/2b/2bEDresult.xlsx
+++ b/logs/2b/2bEDresult.xlsx
@@ -463,14 +463,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>288367.4772720681</v>
+        <v>277758.7223883321</v>
       </c>
     </row>
     <row r="3">
@@ -481,14 +481,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>37077.95610655652</v>
+        <v>37095.81793534155</v>
       </c>
     </row>
     <row r="4">
@@ -499,14 +499,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>76212.74448512004</v>
+        <v>73000.22808200266</v>
       </c>
     </row>
     <row r="5">
@@ -517,14 +517,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>65459.89451755452</v>
+        <v>74934.40562579052</v>
       </c>
     </row>
     <row r="6">
@@ -535,14 +535,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>61483.97985115237</v>
+        <v>60638.74395324037</v>
       </c>
     </row>
     <row r="7">
@@ -553,14 +553,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>197193.9770701673</v>
+        <v>204884.1268372146</v>
       </c>
     </row>
     <row r="8">
@@ -571,14 +571,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>65769.87527668256</v>
+        <v>61273.34275040749</v>
       </c>
     </row>
     <row r="9">
@@ -589,14 +589,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>43470.67566100756</v>
+        <v>45163.13123632164</v>
       </c>
     </row>
     <row r="10">
@@ -607,14 +607,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[7.19709711e+03 1.15587104e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>39902.63259675913</v>
+        <v>35081.65182671895</v>
       </c>
     </row>
     <row r="11">
@@ -625,14 +625,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>63870.64427568849</v>
+        <v>57604.94910536527</v>
       </c>
     </row>
     <row r="12">
@@ -643,14 +643,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>53606.60285983456</v>
+        <v>49366.82860406172</v>
       </c>
     </row>
     <row r="13">
@@ -661,14 +661,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>79141.34638461439</v>
+        <v>84474.65584364621</v>
       </c>
     </row>
     <row r="14">
@@ -679,14 +679,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>44921.95109659878</v>
+        <v>72018.67112973869</v>
       </c>
     </row>
     <row r="15">
@@ -697,14 +697,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>25917.03551715071</v>
+        <v>15213.51750681824</v>
       </c>
     </row>
     <row r="16">
@@ -715,14 +715,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>119147.0126016608</v>
+        <v>114157.8208637684</v>
       </c>
     </row>
     <row r="17">
@@ -733,14 +733,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>110236.8652785443</v>
+        <v>95536.42167269406</v>
       </c>
     </row>
     <row r="18">
@@ -751,14 +751,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>39076.01995699049</v>
+        <v>9185.498507093094</v>
       </c>
     </row>
     <row r="19">
@@ -769,14 +769,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>94435.5860670784</v>
+        <v>77046.91643219895</v>
       </c>
     </row>
     <row r="20">
@@ -787,14 +787,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>57920.27317229209</v>
+        <v>35699.21009542953</v>
       </c>
     </row>
     <row r="21">
@@ -805,14 +805,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>60181.14336261572</v>
+        <v>59062.82087326091</v>
       </c>
     </row>
     <row r="22">
@@ -823,14 +823,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>49375.72487744603</v>
+        <v>43019.26656046376</v>
       </c>
     </row>
     <row r="23">
@@ -841,14 +841,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>28285.22559798326</v>
+        <v>37741.34373458368</v>
       </c>
     </row>
     <row r="24">
@@ -859,14 +859,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D24" t="n">
-        <v>88720.78383139563</v>
+        <v>83068.12708666816</v>
       </c>
     </row>
     <row r="25">
@@ -877,14 +877,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>88691.07082027558</v>
+        <v>79870.8988182763</v>
       </c>
     </row>
     <row r="26">
@@ -895,14 +895,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>10809.82075101969</v>
+        <v>9683.400066965974</v>
       </c>
     </row>
     <row r="27">
@@ -913,14 +913,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>51962.22115294072</v>
+        <v>47638.24049316208</v>
       </c>
     </row>
     <row r="28">
@@ -931,14 +931,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>56632.35964793234</v>
+        <v>51242.75446317265</v>
       </c>
     </row>
     <row r="29">
@@ -949,14 +949,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>64311.88138495572</v>
+        <v>69601.11416828084</v>
       </c>
     </row>
     <row r="30">
@@ -967,14 +967,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>92588.30569530975</v>
+        <v>75205.75338027626</v>
       </c>
     </row>
     <row r="31">
@@ -985,14 +985,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>172064.0270759694</v>
+        <v>176561.2084331697</v>
       </c>
     </row>
     <row r="32">
@@ -1003,14 +1003,14 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>68881.9890500998</v>
+        <v>66980.78941181481</v>
       </c>
     </row>
     <row r="33">
@@ -1021,14 +1021,14 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>52162.87199629247</v>
+        <v>60061.78754944562</v>
       </c>
     </row>
     <row r="34">
@@ -1039,14 +1039,14 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>104200.8998149732</v>
+        <v>91803.28803499766</v>
       </c>
     </row>
     <row r="35">
@@ -1057,14 +1057,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>103711.1430210927</v>
+        <v>107049.2238333962</v>
       </c>
     </row>
     <row r="36">
@@ -1075,14 +1075,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>49696.310961654</v>
+        <v>83751.75461998623</v>
       </c>
     </row>
     <row r="37">
@@ -1093,14 +1093,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>78857.40510303143</v>
+        <v>71461.43734057454</v>
       </c>
     </row>
     <row r="38">
@@ -1111,14 +1111,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>75245.90463842254</v>
+        <v>79944.72260113337</v>
       </c>
     </row>
     <row r="39">
@@ -1129,14 +1129,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C39" t="n">
         <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>36574.67415837741</v>
+        <v>17219.47113380872</v>
       </c>
     </row>
     <row r="40">
@@ -1147,14 +1147,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>232584.7279415662</v>
+        <v>221170.6231690038</v>
       </c>
     </row>
     <row r="41">
@@ -1165,14 +1165,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>92775.39762707532</v>
+        <v>86684.77891563778</v>
       </c>
     </row>
     <row r="42">
@@ -1183,14 +1183,14 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>50010.07821274639</v>
+        <v>43663.32125451612</v>
       </c>
     </row>
     <row r="43">
@@ -1201,14 +1201,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>68941.32044943035</v>
+        <v>55607.52653523351</v>
       </c>
     </row>
     <row r="44">
@@ -1219,14 +1219,14 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C44" t="n">
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>41373.39558683032</v>
+        <v>35333.85466789606</v>
       </c>
     </row>
     <row r="45">
@@ -1237,14 +1237,14 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>153835.6891296762</v>
+        <v>117296.1189971807</v>
       </c>
     </row>
     <row r="46">
@@ -1255,14 +1255,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>21056.24899020842</v>
+        <v>11962.77315853258</v>
       </c>
     </row>
     <row r="47">
@@ -1273,14 +1273,14 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>60845.18985472983</v>
+        <v>46171.65499243356</v>
       </c>
     </row>
     <row r="48">
@@ -1291,14 +1291,14 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C48" t="n">
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>52418.83450274901</v>
+        <v>38035.62015963574</v>
       </c>
     </row>
     <row r="49">
@@ -1309,14 +1309,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>67155.02617346362</v>
+        <v>48690.36232334385</v>
       </c>
     </row>
     <row r="50">
@@ -1327,14 +1327,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>86728.61433369934</v>
+        <v>97724.07439159305</v>
       </c>
     </row>
     <row r="51">
@@ -1345,14 +1345,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D51" t="n">
-        <v>28033.28927197239</v>
+        <v>44214.36370523048</v>
       </c>
     </row>
     <row r="52">
@@ -1363,14 +1363,14 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
-        <v>66964.8029980002</v>
+        <v>52727.87015072416</v>
       </c>
     </row>
     <row r="53">
@@ -1381,14 +1381,14 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>105459.35500033</v>
+        <v>98591.11520209833</v>
       </c>
     </row>
     <row r="54">
@@ -1399,14 +1399,14 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D54" t="n">
-        <v>38135.45955285399</v>
+        <v>31885.51575506464</v>
       </c>
     </row>
     <row r="55">
@@ -1417,14 +1417,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C55" t="n">
         <v>2</v>
       </c>
       <c r="D55" t="n">
-        <v>45031.87239791624</v>
+        <v>28541.95794540149</v>
       </c>
     </row>
     <row r="56">
@@ -1435,14 +1435,14 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>41680.23091614997</v>
+        <v>24418.35780972267</v>
       </c>
     </row>
     <row r="57">
@@ -1453,14 +1453,14 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>180953.1077975127</v>
+        <v>179251.7078405925</v>
       </c>
     </row>
     <row r="58">
@@ -1471,14 +1471,14 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D58" t="n">
-        <v>44240.77138957946</v>
+        <v>40073.27364609123</v>
       </c>
     </row>
     <row r="59">
@@ -1489,14 +1489,14 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>11141.02158185015</v>
+        <v>16453.92820032692</v>
       </c>
     </row>
     <row r="60">
@@ -1507,14 +1507,14 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60" t="n">
-        <v>67652.41714082111</v>
+        <v>63005.16872440478</v>
       </c>
     </row>
     <row r="61">
@@ -1525,14 +1525,14 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>118424.1959187392</v>
+        <v>106094.0269271944</v>
       </c>
     </row>
     <row r="62">
@@ -1543,14 +1543,14 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D62" t="n">
-        <v>198371.8362127496</v>
+        <v>205068.3568461335</v>
       </c>
     </row>
     <row r="63">
@@ -1561,14 +1561,14 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C63" t="n">
         <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>33441.87114001076</v>
+        <v>23711.19223469764</v>
       </c>
     </row>
     <row r="64">
@@ -1579,14 +1579,14 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>214674.1957065134</v>
+        <v>210947.7401439276</v>
       </c>
     </row>
     <row r="65">
@@ -1597,14 +1597,14 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C65" t="n">
         <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>127232.1754430995</v>
+        <v>106194.0853521466</v>
       </c>
     </row>
     <row r="66">
@@ -1615,14 +1615,14 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>76766.87167936935</v>
+        <v>79636.98404194022</v>
       </c>
     </row>
     <row r="67">
@@ -1633,14 +1633,14 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D67" t="n">
-        <v>77647.08824393428</v>
+        <v>79855.710096422</v>
       </c>
     </row>
     <row r="68">
@@ -1651,14 +1651,14 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>37961.6577278872</v>
+        <v>46937.415984216</v>
       </c>
     </row>
     <row r="69">
@@ -1669,14 +1669,14 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>70827.72015816304</v>
+        <v>63502.56843622653</v>
       </c>
     </row>
     <row r="70">
@@ -1687,14 +1687,14 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70" t="n">
-        <v>97953.09418868735</v>
+        <v>88851.15701476202</v>
       </c>
     </row>
     <row r="71">
@@ -1705,14 +1705,14 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>15640.91230922858</v>
+        <v>24381.9296327654</v>
       </c>
     </row>
     <row r="72">
@@ -1723,14 +1723,14 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
-        <v>139284.9163562482</v>
+        <v>122981.285929413</v>
       </c>
     </row>
     <row r="73">
@@ -1741,14 +1741,14 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>29258.38991783627</v>
+        <v>25868.42340415605</v>
       </c>
     </row>
     <row r="74">
@@ -1759,14 +1759,14 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>39367.12999676132</v>
+        <v>47568.41441824466</v>
       </c>
     </row>
     <row r="75">
@@ -1777,14 +1777,14 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" t="n">
-        <v>216655.626593341</v>
+        <v>205236.4772034612</v>
       </c>
     </row>
     <row r="76">
@@ -1795,14 +1795,14 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D76" t="n">
-        <v>31234.71105837398</v>
+        <v>33370.46508597276</v>
       </c>
     </row>
     <row r="77">
@@ -1813,14 +1813,14 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>60401.06638829967</v>
+        <v>77395.74779519942</v>
       </c>
     </row>
     <row r="78">
@@ -1831,14 +1831,14 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D78" t="n">
-        <v>44666.65446389644</v>
+        <v>44937.68992996948</v>
       </c>
     </row>
     <row r="79">
@@ -1849,14 +1849,14 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C79" t="n">
         <v>2</v>
       </c>
       <c r="D79" t="n">
-        <v>79782.76892680538</v>
+        <v>65503.85865760916</v>
       </c>
     </row>
     <row r="80">
@@ -1867,14 +1867,14 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C80" t="n">
         <v>2</v>
       </c>
       <c r="D80" t="n">
-        <v>106592.8711574247</v>
+        <v>87092.15693450019</v>
       </c>
     </row>
     <row r="81">
@@ -1885,14 +1885,14 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C81" t="n">
         <v>2</v>
       </c>
       <c r="D81" t="n">
-        <v>48855.45638476908</v>
+        <v>39470.19796585547</v>
       </c>
     </row>
     <row r="82">
@@ -1903,14 +1903,14 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D82" t="n">
-        <v>145478.1271578487</v>
+        <v>138307.8629632023</v>
       </c>
     </row>
     <row r="83">
@@ -1921,14 +1921,14 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C83" t="n">
         <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>46906.40004208446</v>
+        <v>44410.50179172862</v>
       </c>
     </row>
     <row r="84">
@@ -1939,14 +1939,14 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84" t="n">
-        <v>31345.98475778665</v>
+        <v>25770.4679981156</v>
       </c>
     </row>
     <row r="85">
@@ -1957,14 +1957,14 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[3.74388063e+03 2.03925663e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>8948.975227322953</v>
+        <v>15604.27066347736</v>
       </c>
     </row>
     <row r="86">
@@ -1975,14 +1975,14 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D86" t="n">
-        <v>170780.7311361082</v>
+        <v>187137.3819399667</v>
       </c>
     </row>
     <row r="87">
@@ -1993,14 +1993,14 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C87" t="n">
         <v>2</v>
       </c>
       <c r="D87" t="n">
-        <v>104618.4617020494</v>
+        <v>84999.26106579963</v>
       </c>
     </row>
     <row r="88">
@@ -2011,14 +2011,14 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D88" t="n">
-        <v>86936.0566561086</v>
+        <v>78495.54782598004</v>
       </c>
     </row>
     <row r="89">
@@ -2029,14 +2029,14 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D89" t="n">
-        <v>24688.24964194044</v>
+        <v>27282.47171795214</v>
       </c>
     </row>
     <row r="90">
@@ -2047,14 +2047,14 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="n">
-        <v>42330.16869972117</v>
+        <v>43281.69155146041</v>
       </c>
     </row>
     <row r="91">
@@ -2065,14 +2065,14 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C91" t="n">
         <v>2</v>
       </c>
       <c r="D91" t="n">
-        <v>148299.5613690495</v>
+        <v>137738.2217997131</v>
       </c>
     </row>
     <row r="92">
@@ -2083,14 +2083,14 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[7.19709711e+03 1.15587104e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>172395.0925058125</v>
+        <v>55234.04967519033</v>
       </c>
     </row>
     <row r="93">
@@ -2101,14 +2101,14 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>47127.73662909218</v>
+        <v>39846.34885941728</v>
       </c>
     </row>
     <row r="94">
@@ -2119,14 +2119,14 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>65368.67115951717</v>
+        <v>72514.47824303556</v>
       </c>
     </row>
     <row r="95">
@@ -2137,14 +2137,14 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D95" t="n">
-        <v>60702.9677307723</v>
+        <v>53984.99448686153</v>
       </c>
     </row>
     <row r="96">
@@ -2155,14 +2155,14 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[7.19709711e+03 1.15587104e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C96" t="n">
         <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>221459.410616386</v>
+        <v>357550.9776234818</v>
       </c>
     </row>
     <row r="97">
@@ -2173,14 +2173,14 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[4.83742172e+03 3.84123682e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>83139.05015245725</v>
+        <v>114463.9306521216</v>
       </c>
     </row>
     <row r="98">
@@ -2191,14 +2191,14 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D98" t="n">
-        <v>57231.97750862454</v>
+        <v>53782.25249196319</v>
       </c>
     </row>
     <row r="99">
@@ -2209,14 +2209,14 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99" t="n">
-        <v>66622.29559889676</v>
+        <v>64530.45702431234</v>
       </c>
     </row>
     <row r="100">
@@ -2227,14 +2227,14 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[5.42640895e+03 2.61704610e-03]</t>
+          <t>[4.99026059e+03 2.36094685e-03]</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D100" t="n">
-        <v>3319.369719238799</v>
+        <v>3173.094713420527</v>
       </c>
     </row>
     <row r="101">
@@ -2245,14 +2245,14 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[4.68007750e+03 2.41256204e-03]</t>
+          <t>[4.51499768e+03 2.60946757e-03]</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D101" t="n">
-        <v>61042.32293171186</v>
+        <v>57156.38835851256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>